<commit_message>
aula sobre problemas de transporte de rede
</commit_message>
<xml_diff>
--- a/PesquisaOperacional/2/aula0530/problemaDeRede.xlsx
+++ b/PesquisaOperacional/2/aula0530/problemaDeRede.xlsx
@@ -141,15 +141,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -160,6 +151,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -447,341 +447,335 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>25</v>
       </c>
-      <c r="F4" s="2">
-        <v>50</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <f>SUMIF($C$4:$C$15,H4,$F$4:$F$15)-SUMIF($A$4:$A$15,H4,$F$4:$F$15)</f>
-        <v>-1050</v>
-      </c>
-      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
         <v>-2000</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>20</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>2</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <f t="shared" ref="J5:J10" si="0">SUMIF($C$4:$C$15,H5,$F$4:$F$15)-SUMIF($A$4:$A$15,H5,$F$4:$F$15)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>-3000</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>30</v>
       </c>
-      <c r="F6" s="2">
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>-1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
+        <v>30</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
         <v>1000</v>
       </c>
-      <c r="H6" s="2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1">
+        <v>25</v>
+      </c>
+      <c r="H10" s="1">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="1">
+        <f>SUM(K4:K10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>3</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>-1500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2">
-        <v>30</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2">
-        <v>25</v>
-      </c>
-      <c r="H9" s="2">
-        <v>6</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="2">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2">
-        <v>25</v>
-      </c>
-      <c r="H10" s="2">
-        <v>7</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>2</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2">
-        <f>SUM(K4:K10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>20</v>
       </c>
       <c r="H12" s="9" t="s">
@@ -789,69 +783,69 @@
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="8">
+      <c r="K12" s="5">
         <f>SUMPRODUCT(E4:E15,F4:F15)</f>
-        <v>31250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>5</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>6</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>7</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="5">
         <f>SUMPRODUCT(F4:F15)</f>
-        <v>1050</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -861,12 +855,12 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="H2:H3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>